<commit_message>
add: new function codelco
</commit_message>
<xml_diff>
--- a/output/JAL/importar tottus.xlsx
+++ b/output/JAL/importar tottus.xlsx
@@ -921,7 +921,7 @@
       <c r="AA2" t="inlineStr"/>
       <c r="AB2" t="inlineStr">
         <is>
-          <t>5265</t>
+          <t>8762</t>
         </is>
       </c>
     </row>
@@ -991,7 +991,7 @@
       <c r="AA3" t="inlineStr"/>
       <c r="AB3" t="inlineStr">
         <is>
-          <t>5265</t>
+          <t>8762</t>
         </is>
       </c>
     </row>
@@ -1061,7 +1061,7 @@
       <c r="AA4" t="inlineStr"/>
       <c r="AB4" t="inlineStr">
         <is>
-          <t>5265</t>
+          <t>8762</t>
         </is>
       </c>
     </row>
@@ -1131,7 +1131,7 @@
       <c r="AA5" t="inlineStr"/>
       <c r="AB5" t="inlineStr">
         <is>
-          <t>5265</t>
+          <t>8762</t>
         </is>
       </c>
     </row>
@@ -1201,7 +1201,7 @@
       <c r="AA6" t="inlineStr"/>
       <c r="AB6" t="inlineStr">
         <is>
-          <t>5265</t>
+          <t>8762</t>
         </is>
       </c>
     </row>
@@ -1271,7 +1271,7 @@
       <c r="AA7" t="inlineStr"/>
       <c r="AB7" t="inlineStr">
         <is>
-          <t>5265</t>
+          <t>8762</t>
         </is>
       </c>
     </row>
@@ -1341,7 +1341,7 @@
       <c r="AA8" t="inlineStr"/>
       <c r="AB8" t="inlineStr">
         <is>
-          <t>5265</t>
+          <t>8762</t>
         </is>
       </c>
     </row>
@@ -1411,7 +1411,7 @@
       <c r="AA9" t="inlineStr"/>
       <c r="AB9" t="inlineStr">
         <is>
-          <t>5265</t>
+          <t>8762</t>
         </is>
       </c>
     </row>
@@ -1481,7 +1481,7 @@
       <c r="AA10" t="inlineStr"/>
       <c r="AB10" t="inlineStr">
         <is>
-          <t>5265</t>
+          <t>8762</t>
         </is>
       </c>
     </row>
@@ -1551,7 +1551,7 @@
       <c r="AA11" t="inlineStr"/>
       <c r="AB11" t="inlineStr">
         <is>
-          <t>5265</t>
+          <t>8762</t>
         </is>
       </c>
     </row>
@@ -1621,7 +1621,7 @@
       <c r="AA12" t="inlineStr"/>
       <c r="AB12" t="inlineStr">
         <is>
-          <t>5265</t>
+          <t>8762</t>
         </is>
       </c>
     </row>
@@ -1691,7 +1691,7 @@
       <c r="AA13" t="inlineStr"/>
       <c r="AB13" t="inlineStr">
         <is>
-          <t>5265</t>
+          <t>8762</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
add new function tottus
</commit_message>
<xml_diff>
--- a/output/JAL/importar tottus.xlsx
+++ b/output/JAL/importar tottus.xlsx
@@ -676,7 +676,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AB13"/>
+  <dimension ref="A1:AB16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B3"/>
@@ -858,12 +858,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>46988488</t>
+          <t>47035710</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>46988488</t>
+          <t>47035710</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -888,12 +888,12 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>20250725</t>
+          <t>20250814</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>20250805</t>
+          <t>20250826</t>
         </is>
       </c>
       <c r="I2" t="inlineStr"/>
@@ -912,7 +912,7 @@
         </is>
       </c>
       <c r="T2" t="n">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="W2" t="inlineStr"/>
       <c r="X2" t="inlineStr"/>
@@ -921,19 +921,19 @@
       <c r="AA2" t="inlineStr"/>
       <c r="AB2" t="inlineStr">
         <is>
-          <t>8762</t>
+          <t>8865</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>46988488</t>
+          <t>47035710</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>46988488</t>
+          <t>47035710</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -958,12 +958,12 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>20250725</t>
+          <t>20250814</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>20250805</t>
+          <t>20250826</t>
         </is>
       </c>
       <c r="I3" t="inlineStr"/>
@@ -978,11 +978,11 @@
       <c r="R3" t="inlineStr"/>
       <c r="S3" t="inlineStr">
         <is>
-          <t>20202336</t>
+          <t>20287252</t>
         </is>
       </c>
       <c r="T3" t="n">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="W3" t="inlineStr"/>
       <c r="X3" t="inlineStr"/>
@@ -991,19 +991,19 @@
       <c r="AA3" t="inlineStr"/>
       <c r="AB3" t="inlineStr">
         <is>
-          <t>8762</t>
+          <t>8865</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>46988488</t>
+          <t>47035710</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>46988488</t>
+          <t>47035710</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -1028,12 +1028,12 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>20250725</t>
+          <t>20250814</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>20250805</t>
+          <t>20250826</t>
         </is>
       </c>
       <c r="I4" t="inlineStr"/>
@@ -1048,11 +1048,11 @@
       <c r="R4" t="inlineStr"/>
       <c r="S4" t="inlineStr">
         <is>
-          <t>20202335</t>
+          <t>20287256</t>
         </is>
       </c>
       <c r="T4" t="n">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="W4" t="inlineStr"/>
       <c r="X4" t="inlineStr"/>
@@ -1061,19 +1061,19 @@
       <c r="AA4" t="inlineStr"/>
       <c r="AB4" t="inlineStr">
         <is>
-          <t>8762</t>
+          <t>8865</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>46988488</t>
+          <t>47035710</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>46988488</t>
+          <t>47035710</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -1098,12 +1098,12 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>20250725</t>
+          <t>20250814</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>20250805</t>
+          <t>20250826</t>
         </is>
       </c>
       <c r="I5" t="inlineStr"/>
@@ -1118,11 +1118,11 @@
       <c r="R5" t="inlineStr"/>
       <c r="S5" t="inlineStr">
         <is>
-          <t>20215632</t>
+          <t>20287253</t>
         </is>
       </c>
       <c r="T5" t="n">
-        <v>228</v>
+        <v>24</v>
       </c>
       <c r="W5" t="inlineStr"/>
       <c r="X5" t="inlineStr"/>
@@ -1131,19 +1131,19 @@
       <c r="AA5" t="inlineStr"/>
       <c r="AB5" t="inlineStr">
         <is>
-          <t>8762</t>
+          <t>8865</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>46988488</t>
+          <t>47035710</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>46988488</t>
+          <t>47035710</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1168,12 +1168,12 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>20250725</t>
+          <t>20250814</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>20250805</t>
+          <t>20250826</t>
         </is>
       </c>
       <c r="I6" t="inlineStr"/>
@@ -1188,11 +1188,11 @@
       <c r="R6" t="inlineStr"/>
       <c r="S6" t="inlineStr">
         <is>
-          <t>20202347</t>
+          <t>20202318</t>
         </is>
       </c>
       <c r="T6" t="n">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="W6" t="inlineStr"/>
       <c r="X6" t="inlineStr"/>
@@ -1201,19 +1201,19 @@
       <c r="AA6" t="inlineStr"/>
       <c r="AB6" t="inlineStr">
         <is>
-          <t>8762</t>
+          <t>8865</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>46988488</t>
+          <t>47035710</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>46988488</t>
+          <t>47035710</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -1238,12 +1238,12 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>20250725</t>
+          <t>20250814</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>20250805</t>
+          <t>20250826</t>
         </is>
       </c>
       <c r="I7" t="inlineStr"/>
@@ -1258,11 +1258,11 @@
       <c r="R7" t="inlineStr"/>
       <c r="S7" t="inlineStr">
         <is>
-          <t>20287251</t>
+          <t>20215632</t>
         </is>
       </c>
       <c r="T7" t="n">
-        <v>24</v>
+        <v>240</v>
       </c>
       <c r="W7" t="inlineStr"/>
       <c r="X7" t="inlineStr"/>
@@ -1271,19 +1271,19 @@
       <c r="AA7" t="inlineStr"/>
       <c r="AB7" t="inlineStr">
         <is>
-          <t>8762</t>
+          <t>8865</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>46988488</t>
+          <t>47035710</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>46988488</t>
+          <t>47035710</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -1308,12 +1308,12 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>20250725</t>
+          <t>20250814</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>20250805</t>
+          <t>20250826</t>
         </is>
       </c>
       <c r="I8" t="inlineStr"/>
@@ -1328,7 +1328,7 @@
       <c r="R8" t="inlineStr"/>
       <c r="S8" t="inlineStr">
         <is>
-          <t>20202309</t>
+          <t>20202336</t>
         </is>
       </c>
       <c r="T8" t="n">
@@ -1341,19 +1341,19 @@
       <c r="AA8" t="inlineStr"/>
       <c r="AB8" t="inlineStr">
         <is>
-          <t>8762</t>
+          <t>8865</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>46988488</t>
+          <t>47035710</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>46988488</t>
+          <t>47035710</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -1378,12 +1378,12 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>20250725</t>
+          <t>20250814</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>20250805</t>
+          <t>20250826</t>
         </is>
       </c>
       <c r="I9" t="inlineStr"/>
@@ -1398,11 +1398,11 @@
       <c r="R9" t="inlineStr"/>
       <c r="S9" t="inlineStr">
         <is>
-          <t>20202318</t>
+          <t>20202335</t>
         </is>
       </c>
       <c r="T9" t="n">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="W9" t="inlineStr"/>
       <c r="X9" t="inlineStr"/>
@@ -1411,19 +1411,19 @@
       <c r="AA9" t="inlineStr"/>
       <c r="AB9" t="inlineStr">
         <is>
-          <t>8762</t>
+          <t>8865</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>46988488</t>
+          <t>47035710</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>46988488</t>
+          <t>47035710</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -1448,12 +1448,12 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>20250725</t>
+          <t>20250814</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>20250805</t>
+          <t>20250826</t>
         </is>
       </c>
       <c r="I10" t="inlineStr"/>
@@ -1468,11 +1468,11 @@
       <c r="R10" t="inlineStr"/>
       <c r="S10" t="inlineStr">
         <is>
-          <t>20202310</t>
+          <t>20202339</t>
         </is>
       </c>
       <c r="T10" t="n">
-        <v>48</v>
+        <v>72</v>
       </c>
       <c r="W10" t="inlineStr"/>
       <c r="X10" t="inlineStr"/>
@@ -1481,19 +1481,19 @@
       <c r="AA10" t="inlineStr"/>
       <c r="AB10" t="inlineStr">
         <is>
-          <t>8762</t>
+          <t>8865</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>46988488</t>
+          <t>47035710</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>46988488</t>
+          <t>47035710</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -1518,12 +1518,12 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>20250725</t>
+          <t>20250814</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>20250805</t>
+          <t>20250826</t>
         </is>
       </c>
       <c r="I11" t="inlineStr"/>
@@ -1538,11 +1538,11 @@
       <c r="R11" t="inlineStr"/>
       <c r="S11" t="inlineStr">
         <is>
-          <t>20215634</t>
+          <t>20202309</t>
         </is>
       </c>
       <c r="T11" t="n">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="W11" t="inlineStr"/>
       <c r="X11" t="inlineStr"/>
@@ -1551,19 +1551,19 @@
       <c r="AA11" t="inlineStr"/>
       <c r="AB11" t="inlineStr">
         <is>
-          <t>8762</t>
+          <t>8865</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>46988488</t>
+          <t>47035710</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>46988488</t>
+          <t>47035710</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -1588,12 +1588,12 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>20250725</t>
+          <t>20250814</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>20250805</t>
+          <t>20250826</t>
         </is>
       </c>
       <c r="I12" t="inlineStr"/>
@@ -1608,11 +1608,11 @@
       <c r="R12" t="inlineStr"/>
       <c r="S12" t="inlineStr">
         <is>
-          <t>20202339</t>
+          <t>20202351</t>
         </is>
       </c>
       <c r="T12" t="n">
-        <v>144</v>
+        <v>24</v>
       </c>
       <c r="W12" t="inlineStr"/>
       <c r="X12" t="inlineStr"/>
@@ -1621,19 +1621,19 @@
       <c r="AA12" t="inlineStr"/>
       <c r="AB12" t="inlineStr">
         <is>
-          <t>8762</t>
+          <t>8865</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>46988488</t>
+          <t>47035710</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>46988488</t>
+          <t>47035710</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -1658,12 +1658,12 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>20250725</t>
+          <t>20250814</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>20250805</t>
+          <t>20250826</t>
         </is>
       </c>
       <c r="I13" t="inlineStr"/>
@@ -1678,11 +1678,11 @@
       <c r="R13" t="inlineStr"/>
       <c r="S13" t="inlineStr">
         <is>
-          <t>20287256</t>
+          <t>20202337</t>
         </is>
       </c>
       <c r="T13" t="n">
-        <v>48</v>
+        <v>12</v>
       </c>
       <c r="W13" t="inlineStr"/>
       <c r="X13" t="inlineStr"/>
@@ -1691,7 +1691,217 @@
       <c r="AA13" t="inlineStr"/>
       <c r="AB13" t="inlineStr">
         <is>
-          <t>8762</t>
+          <t>8865</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>47035710</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>47035710</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>78627210-6</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Hipermercados TOTTUS SA</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>CD TOTTUS</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>CD TOTTUS</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>20250814</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>20250826</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="inlineStr"/>
+      <c r="N14" t="inlineStr"/>
+      <c r="O14" t="inlineStr"/>
+      <c r="P14" t="inlineStr"/>
+      <c r="Q14" t="inlineStr"/>
+      <c r="R14" t="inlineStr"/>
+      <c r="S14" t="inlineStr">
+        <is>
+          <t>20287251</t>
+        </is>
+      </c>
+      <c r="T14" t="n">
+        <v>24</v>
+      </c>
+      <c r="W14" t="inlineStr"/>
+      <c r="X14" t="inlineStr"/>
+      <c r="Y14" t="inlineStr"/>
+      <c r="Z14" t="inlineStr"/>
+      <c r="AA14" t="inlineStr"/>
+      <c r="AB14" t="inlineStr">
+        <is>
+          <t>8865</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>47035710</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>47035710</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>78627210-6</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Hipermercados TOTTUS SA</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>CD TOTTUS</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>CD TOTTUS</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>20250814</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>20250826</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="inlineStr"/>
+      <c r="K15" t="inlineStr"/>
+      <c r="L15" t="inlineStr"/>
+      <c r="M15" t="inlineStr"/>
+      <c r="N15" t="inlineStr"/>
+      <c r="O15" t="inlineStr"/>
+      <c r="P15" t="inlineStr"/>
+      <c r="Q15" t="inlineStr"/>
+      <c r="R15" t="inlineStr"/>
+      <c r="S15" t="inlineStr">
+        <is>
+          <t>20202310</t>
+        </is>
+      </c>
+      <c r="T15" t="n">
+        <v>12</v>
+      </c>
+      <c r="W15" t="inlineStr"/>
+      <c r="X15" t="inlineStr"/>
+      <c r="Y15" t="inlineStr"/>
+      <c r="Z15" t="inlineStr"/>
+      <c r="AA15" t="inlineStr"/>
+      <c r="AB15" t="inlineStr">
+        <is>
+          <t>8865</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>47035710</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>47035710</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>78627210-6</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Hipermercados TOTTUS SA</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>CD TOTTUS</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>CD TOTTUS</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>20250814</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>20250826</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="inlineStr"/>
+      <c r="K16" t="inlineStr"/>
+      <c r="L16" t="inlineStr"/>
+      <c r="M16" t="inlineStr"/>
+      <c r="N16" t="inlineStr"/>
+      <c r="O16" t="inlineStr"/>
+      <c r="P16" t="inlineStr"/>
+      <c r="Q16" t="inlineStr"/>
+      <c r="R16" t="inlineStr"/>
+      <c r="S16" t="inlineStr">
+        <is>
+          <t>20215634</t>
+        </is>
+      </c>
+      <c r="T16" t="n">
+        <v>48</v>
+      </c>
+      <c r="W16" t="inlineStr"/>
+      <c r="X16" t="inlineStr"/>
+      <c r="Y16" t="inlineStr"/>
+      <c r="Z16" t="inlineStr"/>
+      <c r="AA16" t="inlineStr"/>
+      <c r="AB16" t="inlineStr">
+        <is>
+          <t>8865</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
add: add collahuasi to streamlit
</commit_message>
<xml_diff>
--- a/output/JAL/importar tottus.xlsx
+++ b/output/JAL/importar tottus.xlsx
@@ -921,7 +921,7 @@
       <c r="AA2" t="inlineStr"/>
       <c r="AB2" t="inlineStr">
         <is>
-          <t>7637</t>
+          <t>3536</t>
         </is>
       </c>
     </row>
@@ -991,7 +991,7 @@
       <c r="AA3" t="inlineStr"/>
       <c r="AB3" t="inlineStr">
         <is>
-          <t>7637</t>
+          <t>3536</t>
         </is>
       </c>
     </row>
@@ -1061,7 +1061,7 @@
       <c r="AA4" t="inlineStr"/>
       <c r="AB4" t="inlineStr">
         <is>
-          <t>7637</t>
+          <t>3536</t>
         </is>
       </c>
     </row>
@@ -1131,7 +1131,7 @@
       <c r="AA5" t="inlineStr"/>
       <c r="AB5" t="inlineStr">
         <is>
-          <t>7637</t>
+          <t>3536</t>
         </is>
       </c>
     </row>
@@ -1201,7 +1201,7 @@
       <c r="AA6" t="inlineStr"/>
       <c r="AB6" t="inlineStr">
         <is>
-          <t>7637</t>
+          <t>3536</t>
         </is>
       </c>
     </row>
@@ -1271,7 +1271,7 @@
       <c r="AA7" t="inlineStr"/>
       <c r="AB7" t="inlineStr">
         <is>
-          <t>7637</t>
+          <t>3536</t>
         </is>
       </c>
     </row>
@@ -1341,7 +1341,7 @@
       <c r="AA8" t="inlineStr"/>
       <c r="AB8" t="inlineStr">
         <is>
-          <t>7637</t>
+          <t>3536</t>
         </is>
       </c>
     </row>
@@ -1411,7 +1411,7 @@
       <c r="AA9" t="inlineStr"/>
       <c r="AB9" t="inlineStr">
         <is>
-          <t>7637</t>
+          <t>3536</t>
         </is>
       </c>
     </row>
@@ -1481,7 +1481,7 @@
       <c r="AA10" t="inlineStr"/>
       <c r="AB10" t="inlineStr">
         <is>
-          <t>7637</t>
+          <t>3536</t>
         </is>
       </c>
     </row>
@@ -1551,7 +1551,7 @@
       <c r="AA11" t="inlineStr"/>
       <c r="AB11" t="inlineStr">
         <is>
-          <t>7637</t>
+          <t>3536</t>
         </is>
       </c>
     </row>
@@ -1621,7 +1621,7 @@
       <c r="AA12" t="inlineStr"/>
       <c r="AB12" t="inlineStr">
         <is>
-          <t>7637</t>
+          <t>3536</t>
         </is>
       </c>
     </row>
@@ -1691,7 +1691,7 @@
       <c r="AA13" t="inlineStr"/>
       <c r="AB13" t="inlineStr">
         <is>
-          <t>7637</t>
+          <t>3536</t>
         </is>
       </c>
     </row>
@@ -1761,7 +1761,7 @@
       <c r="AA14" t="inlineStr"/>
       <c r="AB14" t="inlineStr">
         <is>
-          <t>7637</t>
+          <t>3536</t>
         </is>
       </c>
     </row>
@@ -1831,7 +1831,7 @@
       <c r="AA15" t="inlineStr"/>
       <c r="AB15" t="inlineStr">
         <is>
-          <t>7637</t>
+          <t>3536</t>
         </is>
       </c>
     </row>
@@ -1901,7 +1901,7 @@
       <c r="AA16" t="inlineStr"/>
       <c r="AB16" t="inlineStr">
         <is>
-          <t>7637</t>
+          <t>3536</t>
         </is>
       </c>
     </row>

</xml_diff>